<commit_message>
Automate creation of statewide SNOTEL layer, issue #147
The results are used in Current Conditions for snowpack and wildfires.
</commit_message>
<xml_diff>
--- a/workflow/BasinEntities/Agriculture-FoodAndDairies/data/local-food-data.xlsx
+++ b/workflow/BasinEntities/Agriculture-FoodAndDairies/data/local-food-data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="120">
   <si>
     <t>Organization</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Local food access</t>
   </si>
   <si>
-    <t>Local sales and pickup of local food.</t>
-  </si>
-  <si>
     <t>https://www.rekaivery.com/</t>
   </si>
   <si>
@@ -210,9 +207,6 @@
     <t>2229 W Vine Dr, Fort Collins, CO 80521</t>
   </si>
   <si>
-    <t>Farm Stand</t>
-  </si>
-  <si>
     <t>https://raisinroots.com/</t>
   </si>
   <si>
@@ -325,6 +319,72 @@
   </si>
   <si>
     <t>https://longshadowfarm.wixsite.com/longshadow</t>
+  </si>
+  <si>
+    <t>Buena Vida Farm</t>
+  </si>
+  <si>
+    <t>Local farm and christmas trees</t>
+  </si>
+  <si>
+    <t>http://www.buenavidafarm.com/</t>
+  </si>
+  <si>
+    <t>8204 S County Road 3, Fort Collins, CO 80528</t>
+  </si>
+  <si>
+    <t>Compost Queen</t>
+  </si>
+  <si>
+    <t>Local farm</t>
+  </si>
+  <si>
+    <t>Food compost</t>
+  </si>
+  <si>
+    <t>2224 Stonegate Dr. Fort Collins, CO 80525</t>
+  </si>
+  <si>
+    <t>Mail only</t>
+  </si>
+  <si>
+    <t>Farm stand</t>
+  </si>
+  <si>
+    <t>Weekly food composting service</t>
+  </si>
+  <si>
+    <t>Local sales and pickup of local food</t>
+  </si>
+  <si>
+    <t>https://compostqueenfc.com/</t>
+  </si>
+  <si>
+    <t>Bartels Farm</t>
+  </si>
+  <si>
+    <t>Local farm, pumpkins</t>
+  </si>
+  <si>
+    <t>3424 E Douglas Road, Fort Collins, CO 80524</t>
+  </si>
+  <si>
+    <t>https://thebartelsfarm.com/</t>
+  </si>
+  <si>
+    <t>Something from the Farm</t>
+  </si>
+  <si>
+    <t>Pumpkin Farm</t>
+  </si>
+  <si>
+    <t>Pumpkin farm, seasonal</t>
+  </si>
+  <si>
+    <t>8020 S Timberline Rd, Fort Collins, CO 80525</t>
+  </si>
+  <si>
+    <t>http://www.somethingfromthefarm.com/</t>
   </si>
 </sst>
 </file>
@@ -682,10 +742,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -712,10 +772,10 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -732,625 +792,726 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" t="s">
-        <v>79</v>
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2">
+        <v>-105.01335</v>
+      </c>
+      <c r="H2">
+        <v>40.63917</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3">
-        <v>-104.92805</v>
-      </c>
-      <c r="H3">
-        <v>40.594740000000002</v>
+        <v>76</v>
+      </c>
+      <c r="I3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="G4">
-        <v>-105.10187000000001</v>
+        <v>-104.92805</v>
       </c>
       <c r="H4">
-        <v>40.598529999999997</v>
+        <v>40.594740000000002</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="G5">
-        <v>-105.04009000000001</v>
+        <v>-105.10187000000001</v>
       </c>
       <c r="H5">
-        <v>40.472520000000003</v>
+        <v>40.598529999999997</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="I6" t="s">
-        <v>81</v>
+        <v>99</v>
+      </c>
+      <c r="D6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>-104.96259999999999</v>
+      </c>
+      <c r="H6">
+        <v>40.470820000000003</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G7">
-        <v>-105.06211</v>
+        <v>-105.04009000000001</v>
       </c>
       <c r="H7">
-        <v>40.635170000000002</v>
+        <v>40.472520000000003</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
+        <v>106</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="G8">
-        <v>-104.9983</v>
+        <v>-105.03633000000001</v>
       </c>
       <c r="H8">
-        <v>40.450870000000002</v>
+        <v>40.532260000000001</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9">
-        <v>-105.07264000000001</v>
-      </c>
-      <c r="H9">
-        <v>40.604689999999998</v>
+        <v>27</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="I9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" t="s">
-        <v>84</v>
+        <v>31</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="G10">
-        <v>-105.12875</v>
+        <v>-105.06211</v>
       </c>
       <c r="H10">
-        <v>40.57638</v>
+        <v>40.635170000000002</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="G11">
-        <v>-105.08808000000001</v>
+        <v>-104.9983</v>
       </c>
       <c r="H11">
-        <v>40.609119999999997</v>
+        <v>40.450870000000002</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="G12">
-        <v>-105.14035</v>
+        <v>-105.07264000000001</v>
       </c>
       <c r="H12">
-        <v>40.626899999999999</v>
+        <v>40.604689999999998</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="G13">
-        <v>-104.97794</v>
+        <v>-105.12875</v>
       </c>
       <c r="H13">
-        <v>40.596829999999997</v>
+        <v>40.57638</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>97</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="G14">
-        <v>-105.13927</v>
+        <v>-105.08808000000001</v>
       </c>
       <c r="H14">
-        <v>40.296250000000001</v>
+        <v>40.609119999999997</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F15" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="G15">
-        <v>-105.07118</v>
+        <v>-105.14035</v>
       </c>
       <c r="H15">
-        <v>40.419409999999999</v>
+        <v>40.626899999999999</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G16">
-        <v>-105.11465</v>
+        <v>-104.97794</v>
       </c>
       <c r="H16">
-        <v>40.626060000000003</v>
+        <v>40.596829999999997</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="G17">
-        <v>-105.09896999999999</v>
+        <v>-105.13927</v>
       </c>
       <c r="H17">
-        <v>40.537610000000001</v>
+        <v>40.296250000000001</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>20</v>
+      </c>
+      <c r="E18" t="s">
+        <v>34</v>
       </c>
       <c r="F18" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="G18">
-        <v>-105.17259</v>
+        <v>-105.07118</v>
       </c>
       <c r="H18">
-        <v>40.629579999999997</v>
+        <v>40.419409999999999</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G19">
-        <v>-105.11893999999999</v>
+        <v>-105.11465</v>
       </c>
       <c r="H19">
-        <v>40.59581</v>
+        <v>40.626060000000003</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="2">
-        <v>-105.07958000000001</v>
-      </c>
-      <c r="H20" s="2">
-        <v>40.586379999999998</v>
-      </c>
-      <c r="I20" t="s">
-        <v>12</v>
+        <v>54</v>
+      </c>
+      <c r="E20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20">
+        <v>-105.09896999999999</v>
+      </c>
+      <c r="H20">
+        <v>40.537610000000001</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" s="2">
-        <v>-105.06604</v>
-      </c>
-      <c r="H21" s="2">
-        <v>40.566839999999999</v>
+        <v>57</v>
+      </c>
+      <c r="F21" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21">
+        <v>-105.17259</v>
+      </c>
+      <c r="H21">
+        <v>40.629579999999997</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>23</v>
+        <v>59</v>
+      </c>
+      <c r="E22" t="s">
+        <v>107</v>
       </c>
       <c r="F22" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="G22">
-        <v>-105.07745</v>
+        <v>-105.11893999999999</v>
       </c>
       <c r="H22">
-        <v>40.61551</v>
+        <v>40.59581</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E23" t="s">
-        <v>89</v>
-      </c>
-      <c r="F23" t="s">
-        <v>87</v>
-      </c>
-      <c r="G23">
-        <v>-105.04442</v>
-      </c>
-      <c r="H23">
-        <v>40.66648</v>
+        <v>22</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="2">
+        <v>-105.07958000000001</v>
+      </c>
+      <c r="H23" s="2">
+        <v>40.586379999999998</v>
+      </c>
+      <c r="I23" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24">
-        <v>-105.09446</v>
-      </c>
-      <c r="H24">
-        <v>40.58108</v>
+        <v>31</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="2">
+        <v>-105.06604</v>
+      </c>
+      <c r="H24" s="2">
+        <v>40.566839999999999</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>115</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>116</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" t="s">
-        <v>68</v>
-      </c>
-      <c r="G25">
-        <v>-105.17452</v>
-      </c>
-      <c r="H25">
-        <v>40.426810000000003</v>
+        <v>31</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" s="2">
+        <v>-105.01335</v>
+      </c>
+      <c r="H25" s="2">
+        <v>40.63917</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26">
+        <v>-105.07745</v>
+      </c>
+      <c r="H26">
+        <v>40.61551</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27">
+        <v>-105.04442</v>
+      </c>
+      <c r="H27">
+        <v>40.66648</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28">
+        <v>-105.09446</v>
+      </c>
+      <c r="H28">
+        <v>40.58108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29">
+        <v>-105.17452</v>
+      </c>
+      <c r="H29">
+        <v>40.426810000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" t="s">
         <v>70</v>
       </c>
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" t="s">
-        <v>72</v>
-      </c>
-      <c r="G26">
+      <c r="G30">
         <v>-105.11533</v>
       </c>
-      <c r="H26">
+      <c r="H30">
         <v>40.585740000000001</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>

</xml_diff>